<commit_message>
more minimage works and changing embed builder
</commit_message>
<xml_diff>
--- a/locale/locale.xlsx
+++ b/locale/locale.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\Roshan2\locale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4182DE1-53A1-4259-851D-A7A981B88A3E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E213EB42-202B-431D-8CC8-6E7FEEC5CF3D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2456,14 +2456,6 @@
     <t>playercard.title</t>
   </si>
   <si>
-    <t>:credit_card: **&lt;username&gt;**'s player ID Card
-&lt;social_links&gt;</t>
-  </si>
-  <si>
-    <t>:credit_card: Tarjeta de jugador@ de **&lt;username&gt;**
-&lt;social_links&gt;</t>
-  </si>
-  <si>
     <t>profileRegistered</t>
   </si>
   <si>
@@ -3383,6 +3375,12 @@
   </si>
   <si>
     <t>cat_underlords_help</t>
+  </si>
+  <si>
+    <t>:credit_card: **&lt;username&gt;**'s player ID Card</t>
+  </si>
+  <si>
+    <t>:credit_card: Tarjeta de jugador@ de **&lt;username&gt;**</t>
   </si>
 </sst>
 </file>
@@ -3779,8 +3777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C426"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A322" workbookViewId="0">
+      <selection activeCell="C338" sqref="C338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3792,7 +3790,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -3828,10 +3826,10 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="C4" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3894,10 +3892,10 @@
         <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3924,7 +3922,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="B13" t="s">
         <v>31</v>
@@ -3935,7 +3933,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="B14" t="s">
         <v>33</v>
@@ -4045,13 +4043,13 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="B24" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="C24" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -5370,7 +5368,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="B145" t="s">
         <v>336</v>
@@ -5381,10 +5379,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="B146" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="C146" t="s">
         <v>337</v>
@@ -5392,7 +5390,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="B147" t="s">
         <v>336</v>
@@ -5403,10 +5401,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="B148" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="C148" t="s">
         <v>338</v>
@@ -5414,7 +5412,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="B149" t="s">
         <v>336</v>
@@ -5425,13 +5423,13 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B150" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C150" t="s">
         <v>1073</v>
-      </c>
-      <c r="B150" t="s">
-        <v>1074</v>
-      </c>
-      <c r="C150" t="s">
-        <v>1075</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -6096,18 +6094,18 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="B212" s="4" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="C212" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
@@ -6348,7 +6346,7 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B235" t="s">
         <v>525</v>
@@ -6384,7 +6382,7 @@
         <v>533</v>
       </c>
       <c r="B238" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="C238" t="s">
         <v>534</v>
@@ -6502,7 +6500,7 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="B249" t="s">
         <v>560</v>
@@ -6623,7 +6621,7 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="B260" t="s">
         <v>586</v>
@@ -6656,7 +6654,7 @@
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="B263" t="s">
         <v>594</v>
@@ -6667,7 +6665,7 @@
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="B264" t="s">
         <v>596</v>
@@ -6678,7 +6676,7 @@
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="B265" t="s">
         <v>598</v>
@@ -6689,7 +6687,7 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="B266" t="s">
         <v>600</v>
@@ -6700,7 +6698,7 @@
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="B267" t="s">
         <v>602</v>
@@ -7014,7 +7012,7 @@
         <v>681</v>
       </c>
       <c r="C295" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
@@ -7030,7 +7028,7 @@
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="B297" t="s">
         <v>685</v>
@@ -7055,10 +7053,10 @@
         <v>690</v>
       </c>
       <c r="B299" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="C299" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
@@ -7077,7 +7075,7 @@
         <v>694</v>
       </c>
       <c r="B301" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="C301" t="s">
         <v>695</v>
@@ -7096,13 +7094,13 @@
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" s="2" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="B303" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="C303" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
@@ -7165,10 +7163,10 @@
         <v>713</v>
       </c>
       <c r="B309" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="C309" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
@@ -7473,502 +7471,502 @@
         <v>790</v>
       </c>
       <c r="B337" t="s">
-        <v>791</v>
+        <v>1077</v>
       </c>
       <c r="C337" t="s">
-        <v>792</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="B338" t="s">
+        <v>792</v>
+      </c>
+      <c r="C338" t="s">
         <v>793</v>
-      </c>
-      <c r="B338" t="s">
-        <v>794</v>
-      </c>
-      <c r="C338" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" s="2" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="B339" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C339" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" s="2" t="s">
+        <v>795</v>
+      </c>
+      <c r="B340" t="s">
+        <v>796</v>
+      </c>
+      <c r="C340" t="s">
         <v>797</v>
-      </c>
-      <c r="B340" t="s">
-        <v>798</v>
-      </c>
-      <c r="C340" t="s">
-        <v>799</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="B341" t="s">
+        <v>799</v>
+      </c>
+      <c r="C341" t="s">
         <v>800</v>
-      </c>
-      <c r="B341" t="s">
-        <v>801</v>
-      </c>
-      <c r="C341" t="s">
-        <v>802</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="B342" t="s">
+        <v>802</v>
+      </c>
+      <c r="C342" t="s">
         <v>803</v>
-      </c>
-      <c r="B342" t="s">
-        <v>804</v>
-      </c>
-      <c r="C342" t="s">
-        <v>805</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="B343" t="s">
+        <v>805</v>
+      </c>
+      <c r="C343" t="s">
         <v>806</v>
-      </c>
-      <c r="B343" t="s">
-        <v>807</v>
-      </c>
-      <c r="C343" t="s">
-        <v>808</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B344" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="C344" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
+        <v>809</v>
+      </c>
+      <c r="B345" t="s">
+        <v>810</v>
+      </c>
+      <c r="C345" t="s">
         <v>811</v>
-      </c>
-      <c r="B345" t="s">
-        <v>812</v>
-      </c>
-      <c r="C345" t="s">
-        <v>813</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A346" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="B346" t="s">
+        <v>813</v>
+      </c>
+      <c r="C346" t="s">
         <v>814</v>
-      </c>
-      <c r="B346" t="s">
-        <v>815</v>
-      </c>
-      <c r="C346" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A347" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="B347" t="s">
+        <v>816</v>
+      </c>
+      <c r="C347" t="s">
         <v>817</v>
-      </c>
-      <c r="B347" t="s">
-        <v>818</v>
-      </c>
-      <c r="C347" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A348" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="B348" t="s">
+        <v>819</v>
+      </c>
+      <c r="C348" t="s">
         <v>820</v>
-      </c>
-      <c r="B348" t="s">
-        <v>821</v>
-      </c>
-      <c r="C348" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A349" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="B349" t="s">
+        <v>822</v>
+      </c>
+      <c r="C349" t="s">
         <v>823</v>
-      </c>
-      <c r="B349" t="s">
-        <v>824</v>
-      </c>
-      <c r="C349" t="s">
-        <v>825</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A350" s="2" t="s">
+        <v>824</v>
+      </c>
+      <c r="B350" t="s">
+        <v>825</v>
+      </c>
+      <c r="C350" t="s">
         <v>826</v>
-      </c>
-      <c r="B350" t="s">
-        <v>827</v>
-      </c>
-      <c r="C350" t="s">
-        <v>828</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A351" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="B351" t="s">
+        <v>828</v>
+      </c>
+      <c r="C351" t="s">
         <v>829</v>
-      </c>
-      <c r="B351" t="s">
-        <v>830</v>
-      </c>
-      <c r="C351" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A352" s="2" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="B352" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="C352" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A353" s="2" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B353" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="C353" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="B354" t="s">
+        <v>835</v>
+      </c>
+      <c r="C354" t="s">
         <v>836</v>
-      </c>
-      <c r="B354" t="s">
-        <v>837</v>
-      </c>
-      <c r="C354" t="s">
-        <v>838</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A355" s="2" t="s">
+        <v>837</v>
+      </c>
+      <c r="B355" t="s">
+        <v>838</v>
+      </c>
+      <c r="C355" t="s">
         <v>839</v>
-      </c>
-      <c r="B355" t="s">
-        <v>840</v>
-      </c>
-      <c r="C355" t="s">
-        <v>841</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A356" s="2" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="B356" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="C356" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="B357" t="s">
+        <v>843</v>
+      </c>
+      <c r="C357" t="s">
         <v>844</v>
-      </c>
-      <c r="B357" t="s">
-        <v>845</v>
-      </c>
-      <c r="C357" t="s">
-        <v>846</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A358" s="2" t="s">
+        <v>845</v>
+      </c>
+      <c r="B358" t="s">
+        <v>846</v>
+      </c>
+      <c r="C358" t="s">
         <v>847</v>
-      </c>
-      <c r="B358" t="s">
-        <v>848</v>
-      </c>
-      <c r="C358" t="s">
-        <v>849</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359" s="2" t="s">
+        <v>848</v>
+      </c>
+      <c r="B359" t="s">
+        <v>849</v>
+      </c>
+      <c r="C359" t="s">
         <v>850</v>
-      </c>
-      <c r="B359" t="s">
-        <v>851</v>
-      </c>
-      <c r="C359" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" s="2" t="s">
+        <v>851</v>
+      </c>
+      <c r="B360" t="s">
+        <v>852</v>
+      </c>
+      <c r="C360" t="s">
         <v>853</v>
-      </c>
-      <c r="B360" t="s">
-        <v>854</v>
-      </c>
-      <c r="C360" t="s">
-        <v>855</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A361" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="B361" t="s">
+        <v>855</v>
+      </c>
+      <c r="C361" t="s">
         <v>856</v>
-      </c>
-      <c r="B361" t="s">
-        <v>857</v>
-      </c>
-      <c r="C361" t="s">
-        <v>858</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A362" s="2" t="s">
+        <v>857</v>
+      </c>
+      <c r="B362" t="s">
+        <v>858</v>
+      </c>
+      <c r="C362" t="s">
         <v>859</v>
-      </c>
-      <c r="B362" t="s">
-        <v>860</v>
-      </c>
-      <c r="C362" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A363" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="B363" t="s">
+        <v>861</v>
+      </c>
+      <c r="C363" t="s">
         <v>862</v>
-      </c>
-      <c r="B363" t="s">
-        <v>863</v>
-      </c>
-      <c r="C363" t="s">
-        <v>864</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="B364" t="s">
+        <v>864</v>
+      </c>
+      <c r="C364" t="s">
         <v>865</v>
-      </c>
-      <c r="B364" t="s">
-        <v>866</v>
-      </c>
-      <c r="C364" t="s">
-        <v>867</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="B365" t="s">
+        <v>867</v>
+      </c>
+      <c r="C365" t="s">
         <v>868</v>
-      </c>
-      <c r="B365" t="s">
-        <v>869</v>
-      </c>
-      <c r="C365" t="s">
-        <v>870</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="B366" t="s">
+        <v>870</v>
+      </c>
+      <c r="C366" t="s">
         <v>871</v>
-      </c>
-      <c r="B366" t="s">
-        <v>872</v>
-      </c>
-      <c r="C366" t="s">
-        <v>873</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="B367" t="s">
+        <v>873</v>
+      </c>
+      <c r="C367" t="s">
         <v>874</v>
-      </c>
-      <c r="B367" t="s">
-        <v>875</v>
-      </c>
-      <c r="C367" t="s">
-        <v>876</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="B368" t="s">
+        <v>876</v>
+      </c>
+      <c r="C368" t="s">
         <v>877</v>
-      </c>
-      <c r="B368" t="s">
-        <v>878</v>
-      </c>
-      <c r="C368" t="s">
-        <v>879</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="B369" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="C369" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="B370" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C370" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="B371" t="s">
+        <v>881</v>
+      </c>
+      <c r="C371" t="s">
         <v>882</v>
-      </c>
-      <c r="B371" t="s">
-        <v>883</v>
-      </c>
-      <c r="C371" t="s">
-        <v>884</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" s="2" t="s">
+        <v>883</v>
+      </c>
+      <c r="B372" t="s">
+        <v>884</v>
+      </c>
+      <c r="C372" t="s">
         <v>885</v>
-      </c>
-      <c r="B372" t="s">
-        <v>886</v>
-      </c>
-      <c r="C372" t="s">
-        <v>887</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
+        <v>886</v>
+      </c>
+      <c r="B373" t="s">
+        <v>887</v>
+      </c>
+      <c r="C373" t="s">
         <v>888</v>
-      </c>
-      <c r="B373" t="s">
-        <v>889</v>
-      </c>
-      <c r="C373" t="s">
-        <v>890</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
+        <v>889</v>
+      </c>
+      <c r="B374" t="s">
+        <v>890</v>
+      </c>
+      <c r="C374" t="s">
         <v>891</v>
-      </c>
-      <c r="B374" t="s">
-        <v>892</v>
-      </c>
-      <c r="C374" t="s">
-        <v>893</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
+        <v>892</v>
+      </c>
+      <c r="B375" t="s">
+        <v>893</v>
+      </c>
+      <c r="C375" t="s">
         <v>894</v>
-      </c>
-      <c r="B375" t="s">
-        <v>895</v>
-      </c>
-      <c r="C375" t="s">
-        <v>896</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="B376" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="C376" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="B377" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="C377" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" s="2" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="B378" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="C378" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="B379" t="s">
+        <v>902</v>
+      </c>
+      <c r="C379" t="s">
         <v>903</v>
-      </c>
-      <c r="B379" t="s">
-        <v>904</v>
-      </c>
-      <c r="C379" t="s">
-        <v>905</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="B380" t="s">
+        <v>905</v>
+      </c>
+      <c r="C380" t="s">
         <v>906</v>
-      </c>
-      <c r="B380" t="s">
-        <v>907</v>
-      </c>
-      <c r="C380" t="s">
-        <v>908</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" s="2" t="s">
+        <v>907</v>
+      </c>
+      <c r="B381" t="s">
+        <v>908</v>
+      </c>
+      <c r="C381" t="s">
         <v>909</v>
-      </c>
-      <c r="B381" t="s">
-        <v>910</v>
-      </c>
-      <c r="C381" t="s">
-        <v>911</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="B382" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C382" t="s">
         <v>399</v>
@@ -7976,51 +7974,51 @@
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="B383" t="s">
+        <v>913</v>
+      </c>
+      <c r="C383" t="s">
         <v>914</v>
-      </c>
-      <c r="B383" t="s">
-        <v>915</v>
-      </c>
-      <c r="C383" t="s">
-        <v>916</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A384" s="2" t="s">
+        <v>915</v>
+      </c>
+      <c r="B384" t="s">
+        <v>916</v>
+      </c>
+      <c r="C384" t="s">
         <v>917</v>
-      </c>
-      <c r="B384" t="s">
-        <v>918</v>
-      </c>
-      <c r="C384" t="s">
-        <v>919</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A385" s="2" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="B385" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="C385" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="B386" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="C386" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="B387" t="s">
         <v>120</v>
@@ -8031,150 +8029,150 @@
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
+        <v>923</v>
+      </c>
+      <c r="B388" t="s">
+        <v>924</v>
+      </c>
+      <c r="C388" t="s">
         <v>925</v>
-      </c>
-      <c r="B388" t="s">
-        <v>926</v>
-      </c>
-      <c r="C388" t="s">
-        <v>927</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
+        <v>926</v>
+      </c>
+      <c r="B389" t="s">
+        <v>927</v>
+      </c>
+      <c r="C389" t="s">
         <v>928</v>
-      </c>
-      <c r="B389" t="s">
-        <v>929</v>
-      </c>
-      <c r="C389" t="s">
-        <v>930</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
+        <v>929</v>
+      </c>
+      <c r="B390" t="s">
+        <v>930</v>
+      </c>
+      <c r="C390" t="s">
         <v>931</v>
-      </c>
-      <c r="B390" t="s">
-        <v>932</v>
-      </c>
-      <c r="C390" t="s">
-        <v>933</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
+        <v>932</v>
+      </c>
+      <c r="B391" t="s">
+        <v>933</v>
+      </c>
+      <c r="C391" t="s">
         <v>934</v>
-      </c>
-      <c r="B391" t="s">
-        <v>935</v>
-      </c>
-      <c r="C391" t="s">
-        <v>936</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A392" s="2" t="s">
+        <v>935</v>
+      </c>
+      <c r="B392" t="s">
+        <v>936</v>
+      </c>
+      <c r="C392" t="s">
         <v>937</v>
-      </c>
-      <c r="B392" t="s">
-        <v>938</v>
-      </c>
-      <c r="C392" t="s">
-        <v>939</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A393" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="B393" t="s">
+        <v>939</v>
+      </c>
+      <c r="C393" t="s">
         <v>940</v>
-      </c>
-      <c r="B393" t="s">
-        <v>941</v>
-      </c>
-      <c r="C393" t="s">
-        <v>942</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A394" s="2" t="s">
+        <v>941</v>
+      </c>
+      <c r="B394" t="s">
+        <v>942</v>
+      </c>
+      <c r="C394" t="s">
         <v>943</v>
-      </c>
-      <c r="B394" t="s">
-        <v>944</v>
-      </c>
-      <c r="C394" t="s">
-        <v>945</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A395" s="2" t="s">
+        <v>944</v>
+      </c>
+      <c r="B395" t="s">
+        <v>945</v>
+      </c>
+      <c r="C395" t="s">
         <v>946</v>
-      </c>
-      <c r="B395" t="s">
-        <v>947</v>
-      </c>
-      <c r="C395" t="s">
-        <v>948</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A396" s="2" t="s">
+        <v>947</v>
+      </c>
+      <c r="B396" t="s">
+        <v>948</v>
+      </c>
+      <c r="C396" t="s">
         <v>949</v>
-      </c>
-      <c r="B396" t="s">
-        <v>950</v>
-      </c>
-      <c r="C396" t="s">
-        <v>951</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
+        <v>950</v>
+      </c>
+      <c r="B397" t="s">
+        <v>951</v>
+      </c>
+      <c r="C397" t="s">
         <v>952</v>
-      </c>
-      <c r="B397" t="s">
-        <v>953</v>
-      </c>
-      <c r="C397" t="s">
-        <v>954</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A398" s="2" t="s">
+        <v>953</v>
+      </c>
+      <c r="B398" t="s">
+        <v>954</v>
+      </c>
+      <c r="C398" t="s">
         <v>955</v>
-      </c>
-      <c r="B398" t="s">
-        <v>956</v>
-      </c>
-      <c r="C398" t="s">
-        <v>957</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A399" s="2" t="s">
+        <v>956</v>
+      </c>
+      <c r="B399" t="s">
+        <v>957</v>
+      </c>
+      <c r="C399" t="s">
         <v>958</v>
-      </c>
-      <c r="B399" t="s">
-        <v>959</v>
-      </c>
-      <c r="C399" t="s">
-        <v>960</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A400" s="2" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="B400" t="s">
         <v>652</v>
       </c>
       <c r="C400" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A401" s="2" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="B401" t="s">
         <v>562</v>
@@ -8185,284 +8183,284 @@
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A402" s="2" t="s">
+        <v>962</v>
+      </c>
+      <c r="B402" t="s">
+        <v>963</v>
+      </c>
+      <c r="C402" t="s">
         <v>964</v>
-      </c>
-      <c r="B402" t="s">
-        <v>965</v>
-      </c>
-      <c r="C402" t="s">
-        <v>966</v>
       </c>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A403" s="2" t="s">
+        <v>965</v>
+      </c>
+      <c r="B403" t="s">
+        <v>966</v>
+      </c>
+      <c r="C403" t="s">
         <v>967</v>
-      </c>
-      <c r="B403" t="s">
-        <v>968</v>
-      </c>
-      <c r="C403" t="s">
-        <v>969</v>
       </c>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A404" s="2" t="s">
+        <v>968</v>
+      </c>
+      <c r="B404" t="s">
+        <v>969</v>
+      </c>
+      <c r="C404" t="s">
         <v>970</v>
-      </c>
-      <c r="B404" t="s">
-        <v>971</v>
-      </c>
-      <c r="C404" t="s">
-        <v>972</v>
       </c>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A405" s="2" t="s">
+        <v>971</v>
+      </c>
+      <c r="B405" t="s">
+        <v>972</v>
+      </c>
+      <c r="C405" t="s">
         <v>973</v>
-      </c>
-      <c r="B405" t="s">
-        <v>974</v>
-      </c>
-      <c r="C405" t="s">
-        <v>975</v>
       </c>
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A406" s="2" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="B406" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="C406" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A407" s="2" t="s">
+        <v>976</v>
+      </c>
+      <c r="B407" t="s">
+        <v>977</v>
+      </c>
+      <c r="C407" t="s">
         <v>978</v>
-      </c>
-      <c r="B407" t="s">
-        <v>979</v>
-      </c>
-      <c r="C407" t="s">
-        <v>980</v>
       </c>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A408" s="2" t="s">
+        <v>979</v>
+      </c>
+      <c r="B408" t="s">
+        <v>980</v>
+      </c>
+      <c r="C408" t="s">
         <v>981</v>
-      </c>
-      <c r="B408" t="s">
-        <v>982</v>
-      </c>
-      <c r="C408" t="s">
-        <v>983</v>
       </c>
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A409" s="2" t="s">
+        <v>982</v>
+      </c>
+      <c r="B409" t="s">
+        <v>983</v>
+      </c>
+      <c r="C409" t="s">
         <v>984</v>
-      </c>
-      <c r="B409" t="s">
-        <v>985</v>
-      </c>
-      <c r="C409" t="s">
-        <v>986</v>
       </c>
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A410" s="2" t="s">
+        <v>985</v>
+      </c>
+      <c r="B410" t="s">
+        <v>986</v>
+      </c>
+      <c r="C410" t="s">
         <v>987</v>
-      </c>
-      <c r="B410" t="s">
-        <v>988</v>
-      </c>
-      <c r="C410" t="s">
-        <v>989</v>
       </c>
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A411" s="2" t="s">
+        <v>988</v>
+      </c>
+      <c r="B411" t="s">
+        <v>989</v>
+      </c>
+      <c r="C411" t="s">
         <v>990</v>
-      </c>
-      <c r="B411" t="s">
-        <v>991</v>
-      </c>
-      <c r="C411" t="s">
-        <v>992</v>
       </c>
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A412" s="2" t="s">
+        <v>991</v>
+      </c>
+      <c r="B412" t="s">
+        <v>992</v>
+      </c>
+      <c r="C412" t="s">
         <v>993</v>
-      </c>
-      <c r="B412" t="s">
-        <v>994</v>
-      </c>
-      <c r="C412" t="s">
-        <v>995</v>
       </c>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A413" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="B413" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="C413" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A414" s="2" t="s">
+        <v>996</v>
+      </c>
+      <c r="B414" t="s">
+        <v>997</v>
+      </c>
+      <c r="C414" t="s">
         <v>998</v>
-      </c>
-      <c r="B414" t="s">
-        <v>999</v>
-      </c>
-      <c r="C414" t="s">
-        <v>1000</v>
       </c>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A415" s="2" t="s">
+        <v>999</v>
+      </c>
+      <c r="B415" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C415" t="s">
         <v>1001</v>
-      </c>
-      <c r="B415" t="s">
-        <v>1002</v>
-      </c>
-      <c r="C415" t="s">
-        <v>1003</v>
       </c>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A416" s="2" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="B416" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="C416" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A417" s="2" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B417" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C417" t="s">
         <v>1006</v>
-      </c>
-      <c r="B417" t="s">
-        <v>1007</v>
-      </c>
-      <c r="C417" t="s">
-        <v>1008</v>
       </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A418" s="2" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B418" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C418" t="s">
         <v>1009</v>
-      </c>
-      <c r="B418" t="s">
-        <v>1010</v>
-      </c>
-      <c r="C418" t="s">
-        <v>1011</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A419" s="2" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B419" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C419" t="s">
         <v>1012</v>
-      </c>
-      <c r="B419" t="s">
-        <v>1013</v>
-      </c>
-      <c r="C419" t="s">
-        <v>1014</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A420" s="2" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B420" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C420" t="s">
         <v>1015</v>
-      </c>
-      <c r="B420" t="s">
-        <v>1016</v>
-      </c>
-      <c r="C420" t="s">
-        <v>1017</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A421" s="2" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B421" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C421" t="s">
         <v>1018</v>
-      </c>
-      <c r="B421" t="s">
-        <v>1019</v>
-      </c>
-      <c r="C421" t="s">
-        <v>1020</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A422" s="2" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B422" s="4" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C422" t="s">
         <v>1021</v>
-      </c>
-      <c r="B422" s="4" t="s">
-        <v>1022</v>
-      </c>
-      <c r="C422" t="s">
-        <v>1023</v>
       </c>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A423" s="2" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B423" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C423" t="s">
         <v>1024</v>
-      </c>
-      <c r="B423" t="s">
-        <v>1025</v>
-      </c>
-      <c r="C423" t="s">
-        <v>1026</v>
       </c>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A424" s="2" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B424" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C424" t="s">
         <v>1027</v>
-      </c>
-      <c r="B424" t="s">
-        <v>1028</v>
-      </c>
-      <c r="C424" t="s">
-        <v>1029</v>
       </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A425" s="2" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B425" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C425" t="s">
         <v>1030</v>
-      </c>
-      <c r="B425" t="s">
-        <v>1031</v>
-      </c>
-      <c r="C425" t="s">
-        <v>1032</v>
       </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A426" s="2" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B426" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C426" t="s">
         <v>1033</v>
-      </c>
-      <c r="B426" t="s">
-        <v>1034</v>
-      </c>
-      <c r="C426" t="s">
-        <v>1035</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:C3 B1:C1 A296:C296 A295:B295 A236:C237 B235:C235 A25:C144 B13:C14 A250:C259 B249:C249 A261:C262 B260:C260 B263:C267 A298:C298 B297:C297 A304:C308 A310:C338 A309 A268:C294 A239:C248 A238 C238 A11:C12 A10 A300:C300 A299 A302:C302 A301 C301 A340:C405 A339 A5:C9 A4 A407:C426 A406:B406 A213:C226 A181:B181 A151:C180 B145:C145 A228:C234 A227 A182:C210 A20:C23 C148 B147:C147 C146 A15:C19" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:C3 B1:C1 A296:C296 A295:B295 A236:C237 B235:C235 A25:C144 B13:C14 A250:C259 B249:C249 A261:C262 B260:C260 B263:C267 A298:C298 B297:C297 A304:C308 A310:C336 A309 A268:C294 A239:C248 A238 C238 A11:C12 A10 A300:C300 A299 A302:C302 A301 C301 A340:C405 A339 A5:C9 A4 A407:C426 A406:B406 A213:C226 A181:B181 A151:C180 B145:C145 A228:C234 A227 A182:C210 A20:C23 C148 B147:C147 C146 A15:C19 A338:C338 A337" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaning and turn minigame
</commit_message>
<xml_diff>
--- a/locale/locale.xlsx
+++ b/locale/locale.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\Roshan2\locale\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Roshan-Bot\locale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E213EB42-202B-431D-8CC8-6E7FEEC5CF3D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="locale" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="1079">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="1083">
   <si>
     <t/>
   </si>
@@ -892,9 +891,6 @@
   </si>
   <si>
     <t>Dota 2 current patch</t>
-  </si>
-  <si>
-    <t>Parche actual de dota</t>
   </si>
   <si>
     <t>cmd_ping_args</t>
@@ -3382,11 +3378,26 @@
   <si>
     <t>:credit_card: Tarjeta de jugador@ de **&lt;username&gt;**</t>
   </si>
+  <si>
+    <t>cmd_matches+_args</t>
+  </si>
+  <si>
+    <t>cmd_matches+_help</t>
+  </si>
+  <si>
+    <t>Last played matches. R+</t>
+  </si>
+  <si>
+    <t>Últimas partidas jugadas. R+</t>
+  </si>
+  <si>
+    <t>Parche actual de Dota 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3774,11 +3785,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C426"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C428"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A322" workbookViewId="0">
-      <selection activeCell="C338" sqref="C338"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3790,7 +3801,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -3826,10 +3837,10 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="C4" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3892,10 +3903,10 @@
         <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>1052</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>1053</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3922,7 +3933,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="B13" t="s">
         <v>31</v>
@@ -3933,7 +3944,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B14" t="s">
         <v>33</v>
@@ -4043,13 +4054,13 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="B24" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="C24" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -5016,117 +5027,117 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>268</v>
+        <v>1078</v>
       </c>
       <c r="B113" t="s">
-        <v>269</v>
+        <v>238</v>
       </c>
       <c r="C113" t="s">
-        <v>269</v>
+        <v>239</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>270</v>
+        <v>1079</v>
       </c>
       <c r="B114" t="s">
-        <v>271</v>
+        <v>1080</v>
       </c>
       <c r="C114" t="s">
-        <v>272</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B115" t="s">
-        <v>0</v>
+        <v>269</v>
       </c>
       <c r="C115" t="s">
-        <v>0</v>
+        <v>269</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B116" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C116" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B117" t="s">
-        <v>278</v>
+        <v>0</v>
       </c>
       <c r="C117" t="s">
-        <v>278</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B118" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C118" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B119" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C119" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B120" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C120" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B121" t="s">
-        <v>0</v>
+        <v>283</v>
       </c>
       <c r="C121" t="s">
-        <v>0</v>
+        <v>283</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B122" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C122" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B123" t="s">
         <v>0</v>
@@ -5137,106 +5148,106 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B124" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C124" t="s">
-        <v>293</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B125" t="s">
-        <v>238</v>
+        <v>0</v>
       </c>
       <c r="C125" t="s">
-        <v>239</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B126" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C126" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="B127" t="s">
-        <v>0</v>
+        <v>238</v>
       </c>
       <c r="C127" t="s">
-        <v>0</v>
+        <v>239</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B128" t="s">
-        <v>0</v>
+        <v>295</v>
       </c>
       <c r="C128" t="s">
-        <v>0</v>
+        <v>296</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B129" t="s">
-        <v>301</v>
+        <v>0</v>
       </c>
       <c r="C129" t="s">
-        <v>302</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B130" t="s">
-        <v>304</v>
+        <v>0</v>
       </c>
       <c r="C130" t="s">
-        <v>305</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="B131" t="s">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="C131" t="s">
-        <v>0</v>
+        <v>301</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B132" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C132" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="B133" t="s">
         <v>0</v>
@@ -5247,84 +5258,84 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B134" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C134" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B135" t="s">
-        <v>315</v>
+        <v>0</v>
       </c>
       <c r="C135" t="s">
-        <v>315</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="B136" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="C136" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="B137" t="s">
-        <v>191</v>
+        <v>314</v>
       </c>
       <c r="C137" t="s">
-        <v>192</v>
+        <v>314</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B138" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="C138" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B139" t="s">
-        <v>0</v>
+        <v>191</v>
       </c>
       <c r="C139" t="s">
-        <v>0</v>
+        <v>192</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B140" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C140" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B141" t="s">
         <v>0</v>
@@ -5335,480 +5346,480 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="B142" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C142" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B143" t="s">
-        <v>332</v>
+        <v>0</v>
       </c>
       <c r="C143" t="s">
-        <v>332</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="B144" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C144" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>1062</v>
+        <v>330</v>
       </c>
       <c r="B145" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C145" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>1063</v>
+        <v>332</v>
       </c>
       <c r="B146" t="s">
-        <v>1075</v>
+        <v>333</v>
       </c>
       <c r="C146" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B147" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C147" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="B148" t="s">
         <v>1074</v>
       </c>
       <c r="C148" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>1070</v>
+        <v>1063</v>
       </c>
       <c r="B149" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C149" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>1071</v>
+        <v>1064</v>
       </c>
       <c r="B150" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="C150" t="s">
-        <v>1073</v>
+        <v>337</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>339</v>
+        <v>1069</v>
       </c>
       <c r="B151" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="C151" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>342</v>
+        <v>1070</v>
       </c>
       <c r="B152" t="s">
-        <v>343</v>
+        <v>1071</v>
       </c>
       <c r="C152" t="s">
-        <v>281</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="B153" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="C153" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B154" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="C154" t="s">
-        <v>348</v>
+        <v>281</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="B155" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C155" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="B156" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="C156" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="B157" t="s">
-        <v>176</v>
+        <v>349</v>
       </c>
       <c r="C157" t="s">
-        <v>177</v>
+        <v>350</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="B158" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="C158" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="B159" t="s">
-        <v>360</v>
+        <v>176</v>
       </c>
       <c r="C159" t="s">
-        <v>361</v>
+        <v>177</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="B160" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="C160" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="B161" t="s">
+        <v>359</v>
+      </c>
+      <c r="C161" t="s">
         <v>360</v>
-      </c>
-      <c r="C161" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="B162" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="C162" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="B163" t="s">
-        <v>176</v>
+        <v>359</v>
       </c>
       <c r="C163" t="s">
-        <v>177</v>
+        <v>360</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="B164" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C164" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="B165" t="s">
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="C165" t="s">
-        <v>0</v>
+        <v>177</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B166" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C166" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B167" t="s">
-        <v>377</v>
+        <v>0</v>
       </c>
       <c r="C167" t="s">
-        <v>378</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="B168" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="C168" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B169" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C169" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="B170" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C170" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="B171" t="s">
-        <v>0</v>
+        <v>374</v>
       </c>
       <c r="C171" t="s">
-        <v>0</v>
+        <v>374</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="B172" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="C172" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="B173" t="s">
-        <v>391</v>
+        <v>0</v>
       </c>
       <c r="C173" t="s">
-        <v>392</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B174" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="C174" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="B175" t="s">
-        <v>0</v>
+        <v>390</v>
       </c>
       <c r="C175" t="s">
-        <v>0</v>
+        <v>391</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="B176" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="C176" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="B177" t="s">
-        <v>401</v>
+        <v>0</v>
       </c>
       <c r="C177" t="s">
-        <v>392</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B178" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="C178" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="B179" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="C179" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="B180" t="s">
-        <v>380</v>
+        <v>402</v>
       </c>
       <c r="C180" t="s">
-        <v>381</v>
+        <v>403</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B181" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="C181" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="B182" t="s">
-        <v>413</v>
+        <v>379</v>
       </c>
       <c r="C182" t="s">
-        <v>414</v>
+        <v>380</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="B183" t="s">
-        <v>0</v>
+        <v>409</v>
       </c>
       <c r="C183" t="s">
-        <v>0</v>
+        <v>410</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="B184" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="C184" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B185" t="s">
         <v>0</v>
@@ -5819,260 +5830,260 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="B186" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="C186" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B187" t="s">
-        <v>410</v>
+        <v>0</v>
       </c>
       <c r="C187" t="s">
-        <v>411</v>
+        <v>0</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B188" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C188" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="B189" t="s">
-        <v>427</v>
+        <v>409</v>
       </c>
       <c r="C189" t="s">
-        <v>428</v>
+        <v>410</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="B190" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="C190" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="B191" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="C191" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="B192" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="C192" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="B193" t="s">
-        <v>238</v>
+        <v>432</v>
       </c>
       <c r="C193" t="s">
-        <v>239</v>
+        <v>433</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B194" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="C194" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="B195" t="s">
-        <v>443</v>
+        <v>238</v>
       </c>
       <c r="C195" t="s">
-        <v>443</v>
+        <v>239</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="B196" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="C196" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="B197" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="C197" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="B198" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="C198" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="B199" t="s">
-        <v>117</v>
+        <v>447</v>
       </c>
       <c r="C199" t="s">
-        <v>118</v>
+        <v>448</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="B200" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="C200" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="B201" t="s">
-        <v>283</v>
+        <v>117</v>
       </c>
       <c r="C201" t="s">
-        <v>283</v>
+        <v>118</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="B202" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="C202" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="B203" t="s">
-        <v>461</v>
+        <v>283</v>
       </c>
       <c r="C203" t="s">
-        <v>462</v>
+        <v>283</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="B204" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="C204" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="B205" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="C205" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="B206" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="C206" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="B207" t="s">
-        <v>0</v>
+        <v>466</v>
       </c>
       <c r="C207" t="s">
-        <v>0</v>
+        <v>466</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="B208" t="s">
-        <v>421</v>
+        <v>468</v>
       </c>
       <c r="C208" t="s">
-        <v>421</v>
+        <v>469</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B209" t="s">
         <v>0</v>
@@ -6083,100 +6094,100 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="B210" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C210" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>1066</v>
+        <v>472</v>
+      </c>
+      <c r="B211" t="s">
+        <v>0</v>
+      </c>
+      <c r="C211" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>1067</v>
-      </c>
-      <c r="B212" s="4" t="s">
-        <v>927</v>
+        <v>473</v>
+      </c>
+      <c r="B212" t="s">
+        <v>420</v>
       </c>
       <c r="C212" t="s">
-        <v>928</v>
+        <v>420</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="B213" t="s">
-        <v>476</v>
-      </c>
-      <c r="C213" t="s">
-        <v>477</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="B214" t="s">
-        <v>479</v>
+        <v>1066</v>
+      </c>
+      <c r="B214" s="4" t="s">
+        <v>926</v>
       </c>
       <c r="C214" t="s">
-        <v>480</v>
+        <v>927</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="B215" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="C215" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="B216" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="C216" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
       <c r="B217" t="s">
-        <v>0</v>
+        <v>481</v>
       </c>
       <c r="C217" t="s">
-        <v>0</v>
+        <v>482</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="B218" t="s">
-        <v>165</v>
+        <v>484</v>
       </c>
       <c r="C218" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="B219" t="s">
         <v>0</v>
@@ -6187,18 +6198,18 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B220" t="s">
-        <v>492</v>
+        <v>165</v>
       </c>
       <c r="C220" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="B221" t="s">
         <v>0</v>
@@ -6209,100 +6220,100 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="B222" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="C222" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="B223" t="s">
-        <v>499</v>
+        <v>0</v>
       </c>
       <c r="C223" t="s">
-        <v>500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="B224" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="C224" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="B225" t="s">
-        <v>0</v>
+        <v>498</v>
       </c>
       <c r="C225" t="s">
-        <v>0</v>
+        <v>499</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="B226" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="C226" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
-        <v>508</v>
+        <v>503</v>
+      </c>
+      <c r="B227" t="s">
+        <v>0</v>
+      </c>
+      <c r="C227" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="B228" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="C228" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="B229" t="s">
-        <v>238</v>
-      </c>
-      <c r="C229" t="s">
-        <v>239</v>
+        <v>507</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="B230" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="C230" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="B231" t="s">
         <v>238</v>
@@ -6313,2154 +6324,2176 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="B232" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="C232" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="B233" t="s">
-        <v>520</v>
+        <v>238</v>
       </c>
       <c r="C233" t="s">
-        <v>521</v>
+        <v>239</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
       <c r="B234" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
       <c r="C234" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
-        <v>1036</v>
+        <v>518</v>
       </c>
       <c r="B235" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="C235" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="B236" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="C236" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
-        <v>530</v>
+        <v>1035</v>
       </c>
       <c r="B237" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="C237" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="B238" t="s">
-        <v>1051</v>
+        <v>527</v>
       </c>
       <c r="C238" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="B239" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="C239" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="B240" t="s">
-        <v>539</v>
+        <v>1050</v>
       </c>
       <c r="C240" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="B241" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="C241" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="B242" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="C242" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="B243" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="C243" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="B244" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="C244" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="B245" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="C245" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="B246" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="C246" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="B247" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C247" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="B248" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="C248" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
-        <v>1039</v>
+        <v>554</v>
       </c>
       <c r="B249" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="C249" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="B250" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C250" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
-        <v>564</v>
+        <v>1038</v>
       </c>
       <c r="B251" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="C251" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="B252" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="C252" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="B253" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="C253" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
       <c r="B254" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="C254" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
       <c r="B255" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
       <c r="C255" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="B256" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="C256" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="B257" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="C257" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="B258" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="C258" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="B259" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="C259" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
-        <v>1040</v>
+        <v>580</v>
       </c>
       <c r="B260" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="C260" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="B261" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="C261" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
-        <v>591</v>
+        <v>1039</v>
       </c>
       <c r="B262" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
       <c r="C262" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
-        <v>1041</v>
+        <v>587</v>
       </c>
       <c r="B263" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="C263" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
-        <v>1042</v>
+        <v>590</v>
       </c>
       <c r="B264" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="C264" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
       <c r="B265" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="C265" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="B266" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="C266" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
       <c r="B267" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="C267" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
-        <v>604</v>
+        <v>1043</v>
       </c>
       <c r="B268" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="C268" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
-        <v>607</v>
+        <v>1044</v>
       </c>
       <c r="B269" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
       <c r="C269" t="s">
-        <v>609</v>
+        <v>602</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
-        <v>610</v>
+        <v>603</v>
       </c>
       <c r="B270" t="s">
-        <v>611</v>
+        <v>604</v>
       </c>
       <c r="C270" t="s">
-        <v>612</v>
+        <v>605</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
-        <v>613</v>
+        <v>606</v>
       </c>
       <c r="B271" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
       <c r="C271" t="s">
-        <v>615</v>
+        <v>608</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
       <c r="B272" t="s">
-        <v>617</v>
+        <v>610</v>
       </c>
       <c r="C272" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
       <c r="B273" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="C273" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
       <c r="B274" t="s">
-        <v>623</v>
+        <v>616</v>
       </c>
       <c r="C274" t="s">
-        <v>624</v>
+        <v>617</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
-        <v>625</v>
+        <v>618</v>
       </c>
       <c r="B275" t="s">
-        <v>626</v>
+        <v>619</v>
       </c>
       <c r="C275" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
       <c r="B276" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
       <c r="C276" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
       <c r="B277" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
       <c r="C277" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
-        <v>634</v>
+        <v>627</v>
       </c>
       <c r="B278" t="s">
-        <v>635</v>
+        <v>628</v>
       </c>
       <c r="C278" t="s">
-        <v>636</v>
+        <v>629</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
-        <v>637</v>
+        <v>630</v>
       </c>
       <c r="B279" t="s">
-        <v>638</v>
+        <v>631</v>
       </c>
       <c r="C279" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
-        <v>640</v>
+        <v>633</v>
       </c>
       <c r="B280" t="s">
-        <v>641</v>
+        <v>634</v>
       </c>
       <c r="C280" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="B281" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="C281" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="B282" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="C282" t="s">
-        <v>647</v>
+        <v>640</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
-        <v>648</v>
+        <v>641</v>
       </c>
       <c r="B283" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
       <c r="C283" t="s">
-        <v>650</v>
+        <v>643</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
       <c r="B284" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
       <c r="C284" t="s">
-        <v>653</v>
+        <v>646</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
       <c r="B285" t="s">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="C285" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="B286" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
       <c r="C286" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="B287" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="C287" t="s">
-        <v>661</v>
+        <v>654</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="B288" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
       <c r="C288" t="s">
-        <v>664</v>
+        <v>657</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
-        <v>665</v>
+        <v>658</v>
       </c>
       <c r="B289" t="s">
-        <v>666</v>
+        <v>659</v>
       </c>
       <c r="C289" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="B290" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
       <c r="C290" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
       <c r="B291" t="s">
-        <v>671</v>
+        <v>665</v>
       </c>
       <c r="C291" t="s">
-        <v>671</v>
+        <v>665</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
-        <v>672</v>
+        <v>666</v>
       </c>
       <c r="B292" t="s">
-        <v>673</v>
+        <v>667</v>
       </c>
       <c r="C292" t="s">
-        <v>674</v>
+        <v>668</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
       <c r="B293" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
       <c r="C293" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
       <c r="B294" t="s">
-        <v>678</v>
+        <v>672</v>
       </c>
       <c r="C294" t="s">
-        <v>679</v>
+        <v>673</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
-        <v>680</v>
+        <v>674</v>
       </c>
       <c r="B295" t="s">
-        <v>681</v>
+        <v>675</v>
       </c>
       <c r="C295" t="s">
-        <v>1035</v>
+        <v>675</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
-        <v>682</v>
+        <v>676</v>
       </c>
       <c r="B296" t="s">
-        <v>683</v>
+        <v>677</v>
       </c>
       <c r="C296" t="s">
-        <v>684</v>
+        <v>678</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
-        <v>1046</v>
+        <v>679</v>
       </c>
       <c r="B297" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="C297" t="s">
-        <v>686</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
-        <v>687</v>
+        <v>681</v>
       </c>
       <c r="B298" t="s">
-        <v>688</v>
+        <v>682</v>
       </c>
       <c r="C298" t="s">
-        <v>689</v>
+        <v>683</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
-        <v>690</v>
+        <v>1045</v>
       </c>
       <c r="B299" t="s">
-        <v>1054</v>
+        <v>684</v>
       </c>
       <c r="C299" t="s">
-        <v>1055</v>
+        <v>685</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="B300" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
       <c r="C300" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="B301" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="C301" t="s">
-        <v>695</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" s="2" t="s">
-        <v>696</v>
+        <v>690</v>
       </c>
       <c r="B302" t="s">
-        <v>697</v>
+        <v>691</v>
       </c>
       <c r="C302" t="s">
-        <v>698</v>
+        <v>692</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" s="2" t="s">
-        <v>1057</v>
+        <v>693</v>
       </c>
       <c r="B303" t="s">
-        <v>1048</v>
+        <v>1055</v>
       </c>
       <c r="C303" t="s">
-        <v>1047</v>
+        <v>694</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="B304" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="C304" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
-        <v>702</v>
+        <v>1056</v>
       </c>
       <c r="B305" t="s">
-        <v>703</v>
+        <v>1047</v>
       </c>
       <c r="C305" t="s">
-        <v>704</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" s="2" t="s">
-        <v>705</v>
+        <v>698</v>
       </c>
       <c r="B306" t="s">
-        <v>706</v>
+        <v>699</v>
       </c>
       <c r="C306" t="s">
-        <v>707</v>
+        <v>700</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
-        <v>708</v>
+        <v>701</v>
       </c>
       <c r="B307" t="s">
-        <v>709</v>
+        <v>702</v>
       </c>
       <c r="C307" t="s">
-        <v>709</v>
+        <v>703</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" s="2" t="s">
-        <v>710</v>
+        <v>704</v>
       </c>
       <c r="B308" t="s">
-        <v>711</v>
+        <v>705</v>
       </c>
       <c r="C308" t="s">
-        <v>712</v>
+        <v>706</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" s="2" t="s">
-        <v>713</v>
+        <v>707</v>
       </c>
       <c r="B309" t="s">
-        <v>1050</v>
+        <v>708</v>
       </c>
       <c r="C309" t="s">
-        <v>1049</v>
+        <v>708</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" s="2" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="B310" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="C310" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" s="2" t="s">
-        <v>717</v>
+        <v>712</v>
       </c>
       <c r="B311" t="s">
-        <v>718</v>
+        <v>1049</v>
       </c>
       <c r="C311" t="s">
-        <v>719</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
-        <v>720</v>
+        <v>713</v>
       </c>
       <c r="B312" t="s">
-        <v>721</v>
+        <v>714</v>
       </c>
       <c r="C312" t="s">
-        <v>721</v>
+        <v>715</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
       <c r="B313" t="s">
-        <v>723</v>
+        <v>717</v>
       </c>
       <c r="C313" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
       <c r="B314" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
       <c r="C314" t="s">
-        <v>726</v>
+        <v>720</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
-        <v>727</v>
+        <v>721</v>
       </c>
       <c r="B315" t="s">
-        <v>728</v>
+        <v>722</v>
       </c>
       <c r="C315" t="s">
-        <v>729</v>
+        <v>722</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" s="2" t="s">
-        <v>730</v>
+        <v>723</v>
       </c>
       <c r="B316" t="s">
-        <v>731</v>
+        <v>724</v>
       </c>
       <c r="C316" t="s">
-        <v>732</v>
+        <v>725</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317" s="2" t="s">
-        <v>733</v>
+        <v>726</v>
       </c>
       <c r="B317" t="s">
-        <v>734</v>
+        <v>727</v>
       </c>
       <c r="C317" t="s">
-        <v>735</v>
+        <v>728</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" s="2" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
       <c r="B318" t="s">
-        <v>737</v>
+        <v>730</v>
       </c>
       <c r="C318" t="s">
-        <v>738</v>
+        <v>731</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
-        <v>739</v>
+        <v>732</v>
       </c>
       <c r="B319" t="s">
-        <v>740</v>
+        <v>733</v>
       </c>
       <c r="C319" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
-        <v>742</v>
+        <v>735</v>
       </c>
       <c r="B320" t="s">
-        <v>743</v>
+        <v>736</v>
       </c>
       <c r="C320" t="s">
-        <v>744</v>
+        <v>737</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" s="2" t="s">
-        <v>745</v>
+        <v>738</v>
       </c>
       <c r="B321" t="s">
-        <v>746</v>
+        <v>739</v>
       </c>
       <c r="C321" t="s">
-        <v>747</v>
+        <v>740</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" s="2" t="s">
-        <v>748</v>
+        <v>741</v>
       </c>
       <c r="B322" t="s">
-        <v>749</v>
+        <v>742</v>
       </c>
       <c r="C322" t="s">
-        <v>750</v>
+        <v>743</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" s="2" t="s">
-        <v>751</v>
+        <v>744</v>
       </c>
       <c r="B323" t="s">
-        <v>752</v>
+        <v>745</v>
       </c>
       <c r="C323" t="s">
-        <v>753</v>
+        <v>746</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" s="2" t="s">
-        <v>754</v>
+        <v>747</v>
       </c>
       <c r="B324" t="s">
-        <v>755</v>
+        <v>748</v>
       </c>
       <c r="C324" t="s">
-        <v>756</v>
+        <v>749</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
-        <v>757</v>
+        <v>750</v>
       </c>
       <c r="B325" t="s">
-        <v>758</v>
+        <v>751</v>
       </c>
       <c r="C325" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
-        <v>760</v>
+        <v>753</v>
       </c>
       <c r="B326" t="s">
-        <v>761</v>
+        <v>754</v>
       </c>
       <c r="C326" t="s">
-        <v>761</v>
+        <v>755</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
-        <v>762</v>
+        <v>756</v>
       </c>
       <c r="B327" t="s">
-        <v>763</v>
+        <v>757</v>
       </c>
       <c r="C327" t="s">
-        <v>764</v>
+        <v>758</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" s="2" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="B328" t="s">
-        <v>766</v>
+        <v>760</v>
       </c>
       <c r="C328" t="s">
-        <v>766</v>
+        <v>760</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" s="2" t="s">
-        <v>767</v>
+        <v>761</v>
       </c>
       <c r="B329" t="s">
-        <v>768</v>
+        <v>762</v>
       </c>
       <c r="C329" t="s">
-        <v>769</v>
+        <v>763</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A330" s="2" t="s">
-        <v>770</v>
+        <v>764</v>
       </c>
       <c r="B330" t="s">
-        <v>771</v>
+        <v>765</v>
       </c>
       <c r="C330" t="s">
-        <v>772</v>
+        <v>765</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" s="2" t="s">
-        <v>773</v>
+        <v>766</v>
       </c>
       <c r="B331" t="s">
-        <v>774</v>
+        <v>767</v>
       </c>
       <c r="C331" t="s">
-        <v>775</v>
+        <v>768</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" s="2" t="s">
-        <v>776</v>
+        <v>769</v>
       </c>
       <c r="B332" t="s">
-        <v>777</v>
+        <v>770</v>
       </c>
       <c r="C332" t="s">
-        <v>778</v>
+        <v>771</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" s="2" t="s">
-        <v>779</v>
+        <v>772</v>
       </c>
       <c r="B333" t="s">
-        <v>780</v>
+        <v>773</v>
       </c>
       <c r="C333" t="s">
-        <v>781</v>
+        <v>774</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" s="2" t="s">
-        <v>782</v>
+        <v>775</v>
       </c>
       <c r="B334" t="s">
-        <v>783</v>
+        <v>776</v>
       </c>
       <c r="C334" t="s">
-        <v>784</v>
+        <v>777</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" s="2" t="s">
-        <v>785</v>
+        <v>778</v>
       </c>
       <c r="B335" t="s">
-        <v>786</v>
+        <v>779</v>
       </c>
       <c r="C335" t="s">
-        <v>786</v>
+        <v>780</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" s="2" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="B336" t="s">
-        <v>788</v>
+        <v>782</v>
       </c>
       <c r="C336" t="s">
-        <v>789</v>
+        <v>783</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
-        <v>790</v>
+        <v>784</v>
       </c>
       <c r="B337" t="s">
-        <v>1077</v>
+        <v>785</v>
       </c>
       <c r="C337" t="s">
-        <v>1078</v>
+        <v>785</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="B338" t="s">
-        <v>792</v>
+        <v>787</v>
       </c>
       <c r="C338" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" s="2" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
       <c r="B339" t="s">
-        <v>1058</v>
+        <v>1076</v>
       </c>
       <c r="C339" t="s">
-        <v>1059</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" s="2" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="B340" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
       <c r="C340" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" s="2" t="s">
-        <v>798</v>
+        <v>793</v>
       </c>
       <c r="B341" t="s">
-        <v>799</v>
+        <v>1057</v>
       </c>
       <c r="C341" t="s">
-        <v>800</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" s="2" t="s">
-        <v>801</v>
+        <v>794</v>
       </c>
       <c r="B342" t="s">
-        <v>802</v>
+        <v>795</v>
       </c>
       <c r="C342" t="s">
-        <v>803</v>
+        <v>796</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343" s="2" t="s">
-        <v>804</v>
+        <v>797</v>
       </c>
       <c r="B343" t="s">
-        <v>805</v>
+        <v>798</v>
       </c>
       <c r="C343" t="s">
-        <v>806</v>
+        <v>799</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
-        <v>807</v>
+        <v>800</v>
       </c>
       <c r="B344" t="s">
-        <v>808</v>
+        <v>801</v>
       </c>
       <c r="C344" t="s">
-        <v>808</v>
+        <v>802</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
-        <v>809</v>
+        <v>803</v>
       </c>
       <c r="B345" t="s">
-        <v>810</v>
+        <v>804</v>
       </c>
       <c r="C345" t="s">
-        <v>811</v>
+        <v>805</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A346" s="2" t="s">
-        <v>812</v>
+        <v>806</v>
       </c>
       <c r="B346" t="s">
-        <v>813</v>
+        <v>807</v>
       </c>
       <c r="C346" t="s">
-        <v>814</v>
+        <v>807</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A347" s="2" t="s">
-        <v>815</v>
+        <v>808</v>
       </c>
       <c r="B347" t="s">
-        <v>816</v>
+        <v>809</v>
       </c>
       <c r="C347" t="s">
-        <v>817</v>
+        <v>810</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A348" s="2" t="s">
-        <v>818</v>
+        <v>811</v>
       </c>
       <c r="B348" t="s">
-        <v>819</v>
+        <v>812</v>
       </c>
       <c r="C348" t="s">
-        <v>820</v>
+        <v>813</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A349" s="2" t="s">
-        <v>821</v>
+        <v>814</v>
       </c>
       <c r="B349" t="s">
-        <v>822</v>
+        <v>815</v>
       </c>
       <c r="C349" t="s">
-        <v>823</v>
+        <v>816</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A350" s="2" t="s">
-        <v>824</v>
+        <v>817</v>
       </c>
       <c r="B350" t="s">
-        <v>825</v>
+        <v>818</v>
       </c>
       <c r="C350" t="s">
-        <v>826</v>
+        <v>819</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A351" s="2" t="s">
-        <v>827</v>
+        <v>820</v>
       </c>
       <c r="B351" t="s">
-        <v>828</v>
+        <v>821</v>
       </c>
       <c r="C351" t="s">
-        <v>829</v>
+        <v>822</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A352" s="2" t="s">
-        <v>830</v>
+        <v>823</v>
       </c>
       <c r="B352" t="s">
-        <v>831</v>
+        <v>824</v>
       </c>
       <c r="C352" t="s">
-        <v>831</v>
+        <v>825</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A353" s="2" t="s">
-        <v>832</v>
+        <v>826</v>
       </c>
       <c r="B353" t="s">
-        <v>833</v>
+        <v>827</v>
       </c>
       <c r="C353" t="s">
-        <v>833</v>
+        <v>828</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354" s="2" t="s">
-        <v>834</v>
+        <v>829</v>
       </c>
       <c r="B354" t="s">
-        <v>835</v>
+        <v>830</v>
       </c>
       <c r="C354" t="s">
-        <v>836</v>
+        <v>830</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A355" s="2" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="B355" t="s">
-        <v>838</v>
+        <v>832</v>
       </c>
       <c r="C355" t="s">
-        <v>839</v>
+        <v>832</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A356" s="2" t="s">
-        <v>840</v>
+        <v>833</v>
       </c>
       <c r="B356" t="s">
-        <v>841</v>
+        <v>834</v>
       </c>
       <c r="C356" t="s">
-        <v>841</v>
+        <v>835</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
-        <v>842</v>
+        <v>836</v>
       </c>
       <c r="B357" t="s">
-        <v>843</v>
+        <v>837</v>
       </c>
       <c r="C357" t="s">
-        <v>844</v>
+        <v>838</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A358" s="2" t="s">
-        <v>845</v>
+        <v>839</v>
       </c>
       <c r="B358" t="s">
-        <v>846</v>
+        <v>840</v>
       </c>
       <c r="C358" t="s">
-        <v>847</v>
+        <v>840</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359" s="2" t="s">
-        <v>848</v>
+        <v>841</v>
       </c>
       <c r="B359" t="s">
-        <v>849</v>
+        <v>842</v>
       </c>
       <c r="C359" t="s">
-        <v>850</v>
+        <v>843</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" s="2" t="s">
-        <v>851</v>
+        <v>844</v>
       </c>
       <c r="B360" t="s">
-        <v>852</v>
+        <v>845</v>
       </c>
       <c r="C360" t="s">
-        <v>853</v>
+        <v>846</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A361" s="2" t="s">
-        <v>854</v>
+        <v>847</v>
       </c>
       <c r="B361" t="s">
-        <v>855</v>
+        <v>848</v>
       </c>
       <c r="C361" t="s">
-        <v>856</v>
+        <v>849</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A362" s="2" t="s">
-        <v>857</v>
+        <v>850</v>
       </c>
       <c r="B362" t="s">
-        <v>858</v>
+        <v>851</v>
       </c>
       <c r="C362" t="s">
-        <v>859</v>
+        <v>852</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A363" s="2" t="s">
-        <v>860</v>
+        <v>853</v>
       </c>
       <c r="B363" t="s">
-        <v>861</v>
+        <v>854</v>
       </c>
       <c r="C363" t="s">
-        <v>862</v>
+        <v>855</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
-        <v>863</v>
+        <v>856</v>
       </c>
       <c r="B364" t="s">
-        <v>864</v>
+        <v>857</v>
       </c>
       <c r="C364" t="s">
-        <v>865</v>
+        <v>858</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
-        <v>866</v>
+        <v>859</v>
       </c>
       <c r="B365" t="s">
-        <v>867</v>
+        <v>860</v>
       </c>
       <c r="C365" t="s">
-        <v>868</v>
+        <v>861</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
-        <v>869</v>
+        <v>862</v>
       </c>
       <c r="B366" t="s">
-        <v>870</v>
+        <v>863</v>
       </c>
       <c r="C366" t="s">
-        <v>871</v>
+        <v>864</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
-        <v>872</v>
+        <v>865</v>
       </c>
       <c r="B367" t="s">
-        <v>873</v>
+        <v>866</v>
       </c>
       <c r="C367" t="s">
-        <v>874</v>
+        <v>867</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
-        <v>875</v>
+        <v>868</v>
       </c>
       <c r="B368" t="s">
-        <v>876</v>
+        <v>869</v>
       </c>
       <c r="C368" t="s">
-        <v>877</v>
+        <v>870</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
-        <v>878</v>
+        <v>871</v>
       </c>
       <c r="B369" t="s">
-        <v>867</v>
+        <v>872</v>
       </c>
       <c r="C369" t="s">
-        <v>868</v>
+        <v>873</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
-        <v>879</v>
+        <v>874</v>
       </c>
       <c r="B370" t="s">
-        <v>870</v>
+        <v>875</v>
       </c>
       <c r="C370" t="s">
-        <v>871</v>
+        <v>876</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="B371" t="s">
-        <v>881</v>
+        <v>866</v>
       </c>
       <c r="C371" t="s">
-        <v>882</v>
+        <v>867</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" s="2" t="s">
-        <v>883</v>
+        <v>878</v>
       </c>
       <c r="B372" t="s">
-        <v>884</v>
+        <v>869</v>
       </c>
       <c r="C372" t="s">
-        <v>885</v>
+        <v>870</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
-        <v>886</v>
+        <v>879</v>
       </c>
       <c r="B373" t="s">
-        <v>887</v>
+        <v>880</v>
       </c>
       <c r="C373" t="s">
-        <v>888</v>
+        <v>881</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
-        <v>889</v>
+        <v>882</v>
       </c>
       <c r="B374" t="s">
-        <v>890</v>
+        <v>883</v>
       </c>
       <c r="C374" t="s">
-        <v>891</v>
+        <v>884</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
-        <v>892</v>
+        <v>885</v>
       </c>
       <c r="B375" t="s">
-        <v>893</v>
+        <v>886</v>
       </c>
       <c r="C375" t="s">
-        <v>894</v>
+        <v>887</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
-        <v>895</v>
+        <v>888</v>
       </c>
       <c r="B376" t="s">
-        <v>896</v>
+        <v>889</v>
       </c>
       <c r="C376" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
-        <v>897</v>
+        <v>891</v>
       </c>
       <c r="B377" t="s">
-        <v>898</v>
+        <v>892</v>
       </c>
       <c r="C377" t="s">
-        <v>898</v>
+        <v>893</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" s="2" t="s">
-        <v>899</v>
+        <v>894</v>
       </c>
       <c r="B378" t="s">
-        <v>900</v>
+        <v>895</v>
       </c>
       <c r="C378" t="s">
-        <v>900</v>
+        <v>895</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" s="2" t="s">
-        <v>901</v>
+        <v>896</v>
       </c>
       <c r="B379" t="s">
-        <v>902</v>
+        <v>897</v>
       </c>
       <c r="C379" t="s">
-        <v>903</v>
+        <v>897</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="B380" t="s">
-        <v>905</v>
+        <v>899</v>
       </c>
       <c r="C380" t="s">
-        <v>906</v>
+        <v>899</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" s="2" t="s">
-        <v>907</v>
+        <v>900</v>
       </c>
       <c r="B381" t="s">
-        <v>908</v>
+        <v>901</v>
       </c>
       <c r="C381" t="s">
-        <v>909</v>
+        <v>902</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
-        <v>910</v>
+        <v>903</v>
       </c>
       <c r="B382" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="C382" t="s">
-        <v>399</v>
+        <v>905</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" s="2" t="s">
-        <v>912</v>
+        <v>906</v>
       </c>
       <c r="B383" t="s">
-        <v>913</v>
+        <v>907</v>
       </c>
       <c r="C383" t="s">
-        <v>914</v>
+        <v>908</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A384" s="2" t="s">
-        <v>915</v>
+        <v>909</v>
       </c>
       <c r="B384" t="s">
-        <v>916</v>
+        <v>910</v>
       </c>
       <c r="C384" t="s">
-        <v>917</v>
+        <v>398</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A385" s="2" t="s">
-        <v>918</v>
+        <v>911</v>
       </c>
       <c r="B385" t="s">
-        <v>919</v>
+        <v>912</v>
       </c>
       <c r="C385" t="s">
-        <v>919</v>
+        <v>913</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
-        <v>920</v>
+        <v>914</v>
       </c>
       <c r="B386" t="s">
-        <v>921</v>
+        <v>915</v>
       </c>
       <c r="C386" t="s">
-        <v>921</v>
+        <v>916</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
-        <v>922</v>
+        <v>917</v>
       </c>
       <c r="B387" t="s">
-        <v>120</v>
+        <v>918</v>
       </c>
       <c r="C387" t="s">
-        <v>120</v>
+        <v>918</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
       <c r="B388" t="s">
-        <v>924</v>
+        <v>920</v>
       </c>
       <c r="C388" t="s">
-        <v>925</v>
+        <v>920</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
-        <v>926</v>
+        <v>921</v>
       </c>
       <c r="B389" t="s">
-        <v>927</v>
+        <v>120</v>
       </c>
       <c r="C389" t="s">
-        <v>928</v>
+        <v>120</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
-        <v>929</v>
+        <v>922</v>
       </c>
       <c r="B390" t="s">
-        <v>930</v>
+        <v>923</v>
       </c>
       <c r="C390" t="s">
-        <v>931</v>
+        <v>924</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
-        <v>932</v>
+        <v>925</v>
       </c>
       <c r="B391" t="s">
-        <v>933</v>
+        <v>926</v>
       </c>
       <c r="C391" t="s">
-        <v>934</v>
+        <v>927</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A392" s="2" t="s">
-        <v>935</v>
+        <v>928</v>
       </c>
       <c r="B392" t="s">
-        <v>936</v>
+        <v>929</v>
       </c>
       <c r="C392" t="s">
-        <v>937</v>
+        <v>930</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A393" s="2" t="s">
-        <v>938</v>
+        <v>931</v>
       </c>
       <c r="B393" t="s">
-        <v>939</v>
+        <v>932</v>
       </c>
       <c r="C393" t="s">
-        <v>940</v>
+        <v>933</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A394" s="2" t="s">
-        <v>941</v>
+        <v>934</v>
       </c>
       <c r="B394" t="s">
-        <v>942</v>
+        <v>935</v>
       </c>
       <c r="C394" t="s">
-        <v>943</v>
+        <v>936</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A395" s="2" t="s">
-        <v>944</v>
+        <v>937</v>
       </c>
       <c r="B395" t="s">
-        <v>945</v>
+        <v>938</v>
       </c>
       <c r="C395" t="s">
-        <v>946</v>
+        <v>939</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A396" s="2" t="s">
-        <v>947</v>
+        <v>940</v>
       </c>
       <c r="B396" t="s">
-        <v>948</v>
+        <v>941</v>
       </c>
       <c r="C396" t="s">
-        <v>949</v>
+        <v>942</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
-        <v>950</v>
+        <v>943</v>
       </c>
       <c r="B397" t="s">
-        <v>951</v>
+        <v>944</v>
       </c>
       <c r="C397" t="s">
-        <v>952</v>
+        <v>945</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A398" s="2" t="s">
-        <v>953</v>
+        <v>946</v>
       </c>
       <c r="B398" t="s">
-        <v>954</v>
+        <v>947</v>
       </c>
       <c r="C398" t="s">
-        <v>955</v>
+        <v>948</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A399" s="2" t="s">
-        <v>956</v>
+        <v>949</v>
       </c>
       <c r="B399" t="s">
-        <v>957</v>
+        <v>950</v>
       </c>
       <c r="C399" t="s">
-        <v>958</v>
+        <v>951</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A400" s="2" t="s">
-        <v>959</v>
+        <v>952</v>
       </c>
       <c r="B400" t="s">
-        <v>652</v>
+        <v>953</v>
       </c>
       <c r="C400" t="s">
-        <v>960</v>
+        <v>954</v>
       </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A401" s="2" t="s">
-        <v>961</v>
+        <v>955</v>
       </c>
       <c r="B401" t="s">
-        <v>562</v>
+        <v>956</v>
       </c>
       <c r="C401" t="s">
-        <v>563</v>
+        <v>957</v>
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A402" s="2" t="s">
-        <v>962</v>
+        <v>958</v>
       </c>
       <c r="B402" t="s">
-        <v>963</v>
+        <v>651</v>
       </c>
       <c r="C402" t="s">
-        <v>964</v>
+        <v>959</v>
       </c>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A403" s="2" t="s">
-        <v>965</v>
+        <v>960</v>
       </c>
       <c r="B403" t="s">
-        <v>966</v>
+        <v>561</v>
       </c>
       <c r="C403" t="s">
-        <v>967</v>
+        <v>562</v>
       </c>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A404" s="2" t="s">
-        <v>968</v>
+        <v>961</v>
       </c>
       <c r="B404" t="s">
-        <v>969</v>
+        <v>962</v>
       </c>
       <c r="C404" t="s">
-        <v>970</v>
+        <v>963</v>
       </c>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A405" s="2" t="s">
-        <v>971</v>
+        <v>964</v>
       </c>
       <c r="B405" t="s">
-        <v>972</v>
+        <v>965</v>
       </c>
       <c r="C405" t="s">
-        <v>973</v>
+        <v>966</v>
       </c>
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A406" s="2" t="s">
-        <v>974</v>
+        <v>967</v>
       </c>
       <c r="B406" t="s">
-        <v>975</v>
+        <v>968</v>
       </c>
       <c r="C406" t="s">
-        <v>1061</v>
+        <v>969</v>
       </c>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A407" s="2" t="s">
-        <v>976</v>
+        <v>970</v>
       </c>
       <c r="B407" t="s">
-        <v>977</v>
+        <v>971</v>
       </c>
       <c r="C407" t="s">
-        <v>978</v>
+        <v>972</v>
       </c>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A408" s="2" t="s">
-        <v>979</v>
+        <v>973</v>
       </c>
       <c r="B408" t="s">
-        <v>980</v>
+        <v>974</v>
       </c>
       <c r="C408" t="s">
-        <v>981</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A409" s="2" t="s">
-        <v>982</v>
+        <v>975</v>
       </c>
       <c r="B409" t="s">
-        <v>983</v>
+        <v>976</v>
       </c>
       <c r="C409" t="s">
-        <v>984</v>
+        <v>977</v>
       </c>
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A410" s="2" t="s">
-        <v>985</v>
+        <v>978</v>
       </c>
       <c r="B410" t="s">
-        <v>986</v>
+        <v>979</v>
       </c>
       <c r="C410" t="s">
-        <v>987</v>
+        <v>980</v>
       </c>
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A411" s="2" t="s">
-        <v>988</v>
+        <v>981</v>
       </c>
       <c r="B411" t="s">
-        <v>989</v>
+        <v>982</v>
       </c>
       <c r="C411" t="s">
-        <v>990</v>
+        <v>983</v>
       </c>
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A412" s="2" t="s">
-        <v>991</v>
+        <v>984</v>
       </c>
       <c r="B412" t="s">
-        <v>992</v>
+        <v>985</v>
       </c>
       <c r="C412" t="s">
-        <v>993</v>
+        <v>986</v>
       </c>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A413" s="2" t="s">
-        <v>994</v>
+        <v>987</v>
       </c>
       <c r="B413" t="s">
-        <v>995</v>
+        <v>988</v>
       </c>
       <c r="C413" t="s">
-        <v>995</v>
+        <v>989</v>
       </c>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A414" s="2" t="s">
-        <v>996</v>
+        <v>990</v>
       </c>
       <c r="B414" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="C414" t="s">
-        <v>998</v>
+        <v>992</v>
       </c>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A415" s="2" t="s">
-        <v>999</v>
+        <v>993</v>
       </c>
       <c r="B415" t="s">
-        <v>1000</v>
+        <v>994</v>
       </c>
       <c r="C415" t="s">
-        <v>1001</v>
+        <v>994</v>
       </c>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A416" s="2" t="s">
-        <v>1002</v>
+        <v>995</v>
       </c>
       <c r="B416" t="s">
-        <v>1003</v>
+        <v>996</v>
       </c>
       <c r="C416" t="s">
-        <v>1003</v>
+        <v>997</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A417" s="2" t="s">
-        <v>1004</v>
+        <v>998</v>
       </c>
       <c r="B417" t="s">
-        <v>1005</v>
+        <v>999</v>
       </c>
       <c r="C417" t="s">
-        <v>1006</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A418" s="2" t="s">
-        <v>1007</v>
+        <v>1001</v>
       </c>
       <c r="B418" t="s">
-        <v>1008</v>
+        <v>1002</v>
       </c>
       <c r="C418" t="s">
-        <v>1009</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A419" s="2" t="s">
-        <v>1010</v>
+        <v>1003</v>
       </c>
       <c r="B419" t="s">
-        <v>1011</v>
+        <v>1004</v>
       </c>
       <c r="C419" t="s">
-        <v>1012</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A420" s="2" t="s">
-        <v>1013</v>
+        <v>1006</v>
       </c>
       <c r="B420" t="s">
-        <v>1014</v>
+        <v>1007</v>
       </c>
       <c r="C420" t="s">
-        <v>1015</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A421" s="2" t="s">
-        <v>1016</v>
+        <v>1009</v>
       </c>
       <c r="B421" t="s">
-        <v>1017</v>
+        <v>1010</v>
       </c>
       <c r="C421" t="s">
-        <v>1018</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A422" s="2" t="s">
-        <v>1019</v>
-      </c>
-      <c r="B422" s="4" t="s">
-        <v>1020</v>
+        <v>1012</v>
+      </c>
+      <c r="B422" t="s">
+        <v>1013</v>
       </c>
       <c r="C422" t="s">
-        <v>1021</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A423" s="2" t="s">
-        <v>1022</v>
+        <v>1015</v>
       </c>
       <c r="B423" t="s">
-        <v>1023</v>
+        <v>1016</v>
       </c>
       <c r="C423" t="s">
-        <v>1024</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A424" s="2" t="s">
-        <v>1025</v>
-      </c>
-      <c r="B424" t="s">
-        <v>1026</v>
+        <v>1018</v>
+      </c>
+      <c r="B424" s="4" t="s">
+        <v>1019</v>
       </c>
       <c r="C424" t="s">
-        <v>1027</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A425" s="2" t="s">
-        <v>1028</v>
+        <v>1021</v>
       </c>
       <c r="B425" t="s">
-        <v>1029</v>
+        <v>1022</v>
       </c>
       <c r="C425" t="s">
-        <v>1030</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A426" s="2" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B426" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C426" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="427" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A427" s="2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B427" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C427" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="428" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A428" s="2" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B428" t="s">
         <v>1031</v>
       </c>
-      <c r="B426" t="s">
+      <c r="C428" t="s">
         <v>1032</v>
-      </c>
-      <c r="C426" t="s">
-        <v>1033</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:C3 B1:C1 A296:C296 A295:B295 A236:C237 B235:C235 A25:C144 B13:C14 A250:C259 B249:C249 A261:C262 B260:C260 B263:C267 A298:C298 B297:C297 A304:C308 A310:C336 A309 A268:C294 A239:C248 A238 C238 A11:C12 A10 A300:C300 A299 A302:C302 A301 C301 A340:C405 A339 A5:C9 A4 A407:C426 A406:B406 A213:C226 A181:B181 A151:C180 B145:C145 A228:C234 A227 A182:C210 A20:C23 C148 B147:C147 C146 A15:C19 A338:C338 A337" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:C3 B1:C1 A298:C298 A297:B297 A238:C239 B237:C237 A115:C123 B13:C14 A252:C261 B251:C251 A263:C264 B262:C262 B265:C269 A300:C300 B299:C299 A306:C310 A312:C338 A311 A270:C296 A241:C250 A240 C240 A11:C12 A10 A302:C302 A301 A304:C304 A303 C303 A342:C407 A341 A5:C9 A4 A409:C428 A408:B408 A215:C228 A183:B183 A153:C182 B147:C147 A230:C236 A229 A184:C212 C150 B149:C149 C148 A15:C23 A340:C340 A339 A25:C111 A125:C146 A124:B124 A112:B112" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
help command shows aliases, added 'game' alias to 'match' commands, changes in cache and logger components
</commit_message>
<xml_diff>
--- a/locale/locale.xlsx
+++ b/locale/locale.xlsx
@@ -3074,9 +3074,6 @@
     <t>tourneys.suggestion</t>
   </si>
   <si>
-    <t>Suggest tournamente/event</t>
-  </si>
-  <si>
     <t>Sugerir torneo/evento</t>
   </si>
   <si>
@@ -3449,6 +3446,9 @@
   </si>
   <si>
     <t>Roles</t>
+  </si>
+  <si>
+    <t>Suggest tournament/event</t>
   </si>
 </sst>
 </file>
@@ -3845,8 +3845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C435"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A275" workbookViewId="0">
-      <selection activeCell="C292" sqref="C292"/>
+    <sheetView tabSelected="1" topLeftCell="A398" workbookViewId="0">
+      <selection activeCell="B417" sqref="B417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3858,7 +3858,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -3894,10 +3894,10 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="C4" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3960,10 +3960,10 @@
         <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>1051</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>1052</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3990,29 +3990,29 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B13" t="s">
         <v>1086</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>1087</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1088</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B14" t="s">
         <v>1083</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>1084</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1085</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B15" t="s">
         <v>31</v>
@@ -4023,7 +4023,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="B16" t="s">
         <v>33</v>
@@ -4133,13 +4133,13 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B26" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="C26" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -5106,7 +5106,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B115" t="s">
         <v>238</v>
@@ -5117,13 +5117,13 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B116" t="s">
         <v>1079</v>
       </c>
-      <c r="B116" t="s">
+      <c r="C116" t="s">
         <v>1080</v>
-      </c>
-      <c r="C116" t="s">
-        <v>1081</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -5233,7 +5233,7 @@
         <v>289</v>
       </c>
       <c r="C126" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -5480,7 +5480,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B149" t="s">
         <v>335</v>
@@ -5491,10 +5491,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B150" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="C150" t="s">
         <v>336</v>
@@ -5502,7 +5502,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B151" t="s">
         <v>335</v>
@@ -5513,10 +5513,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="B152" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C152" t="s">
         <v>337</v>
@@ -5524,7 +5524,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="B153" t="s">
         <v>335</v>
@@ -5535,13 +5535,13 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B154" t="s">
         <v>1070</v>
       </c>
-      <c r="B154" t="s">
+      <c r="C154" t="s">
         <v>1071</v>
-      </c>
-      <c r="C154" t="s">
-        <v>1072</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -6206,12 +6206,12 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="B216" s="4" t="s">
         <v>926</v>
@@ -6458,7 +6458,7 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="B239" t="s">
         <v>524</v>
@@ -6494,7 +6494,7 @@
         <v>532</v>
       </c>
       <c r="B242" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="C242" t="s">
         <v>533</v>
@@ -6612,7 +6612,7 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B253" t="s">
         <v>559</v>
@@ -6733,7 +6733,7 @@
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B264" t="s">
         <v>585</v>
@@ -6766,7 +6766,7 @@
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="B267" t="s">
         <v>593</v>
@@ -6777,7 +6777,7 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B268" t="s">
         <v>595</v>
@@ -6788,7 +6788,7 @@
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="B269" t="s">
         <v>597</v>
@@ -6799,7 +6799,7 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="B270" t="s">
         <v>599</v>
@@ -6810,7 +6810,7 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="B271" t="s">
         <v>601</v>
@@ -7041,13 +7041,13 @@
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B292" t="s">
         <v>1100</v>
       </c>
-      <c r="B292" t="s">
-        <v>1101</v>
-      </c>
       <c r="C292" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
@@ -7135,7 +7135,7 @@
         <v>680</v>
       </c>
       <c r="C300" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
@@ -7151,7 +7151,7 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" s="2" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B302" t="s">
         <v>684</v>
@@ -7176,10 +7176,10 @@
         <v>689</v>
       </c>
       <c r="B304" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C304" t="s">
         <v>1053</v>
-      </c>
-      <c r="C304" t="s">
-        <v>1054</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
@@ -7198,7 +7198,7 @@
         <v>693</v>
       </c>
       <c r="B306" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="C306" t="s">
         <v>694</v>
@@ -7217,13 +7217,13 @@
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" s="2" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="B308" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="C308" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
@@ -7286,10 +7286,10 @@
         <v>712</v>
       </c>
       <c r="B314" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="C314" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
@@ -7426,13 +7426,13 @@
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B327" t="s">
         <v>1097</v>
       </c>
-      <c r="B327" t="s">
+      <c r="C327" t="s">
         <v>1098</v>
-      </c>
-      <c r="C327" t="s">
-        <v>1099</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
@@ -7605,10 +7605,10 @@
         <v>789</v>
       </c>
       <c r="B343" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C343" t="s">
         <v>1076</v>
-      </c>
-      <c r="C343" t="s">
-        <v>1077</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.25">
@@ -7627,10 +7627,10 @@
         <v>793</v>
       </c>
       <c r="B345" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C345" t="s">
         <v>1057</v>
-      </c>
-      <c r="C345" t="s">
-        <v>1058</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.25">
@@ -7888,13 +7888,13 @@
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B369" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C369" t="s">
         <v>1089</v>
-      </c>
-      <c r="C369" t="s">
-        <v>1090</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
@@ -8141,24 +8141,24 @@
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A392" s="2" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B392" t="s">
         <v>435</v>
       </c>
       <c r="C392" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A393" s="2" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B393" t="s">
         <v>1094</v>
       </c>
-      <c r="B393" t="s">
+      <c r="C393" t="s">
         <v>1095</v>
-      </c>
-      <c r="C393" t="s">
-        <v>1096</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.25">
@@ -8400,7 +8400,7 @@
         <v>974</v>
       </c>
       <c r="C415" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.25">
@@ -8419,215 +8419,215 @@
         <v>978</v>
       </c>
       <c r="B417" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C417" t="s">
         <v>979</v>
-      </c>
-      <c r="C417" t="s">
-        <v>980</v>
       </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A418" s="2" t="s">
+        <v>980</v>
+      </c>
+      <c r="B418" t="s">
         <v>981</v>
       </c>
-      <c r="B418" t="s">
+      <c r="C418" t="s">
         <v>982</v>
-      </c>
-      <c r="C418" t="s">
-        <v>983</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A419" s="2" t="s">
+        <v>983</v>
+      </c>
+      <c r="B419" t="s">
         <v>984</v>
       </c>
-      <c r="B419" t="s">
+      <c r="C419" t="s">
         <v>985</v>
-      </c>
-      <c r="C419" t="s">
-        <v>986</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A420" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="B420" t="s">
         <v>987</v>
       </c>
-      <c r="B420" t="s">
+      <c r="C420" t="s">
         <v>988</v>
-      </c>
-      <c r="C420" t="s">
-        <v>989</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A421" s="2" t="s">
+        <v>989</v>
+      </c>
+      <c r="B421" t="s">
         <v>990</v>
       </c>
-      <c r="B421" t="s">
+      <c r="C421" t="s">
         <v>991</v>
-      </c>
-      <c r="C421" t="s">
-        <v>992</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A422" s="2" t="s">
+        <v>992</v>
+      </c>
+      <c r="B422" t="s">
         <v>993</v>
       </c>
-      <c r="B422" t="s">
-        <v>994</v>
-      </c>
       <c r="C422" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A423" s="2" t="s">
+        <v>994</v>
+      </c>
+      <c r="B423" t="s">
         <v>995</v>
       </c>
-      <c r="B423" t="s">
+      <c r="C423" t="s">
         <v>996</v>
-      </c>
-      <c r="C423" t="s">
-        <v>997</v>
       </c>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A424" s="2" t="s">
+        <v>997</v>
+      </c>
+      <c r="B424" t="s">
         <v>998</v>
       </c>
-      <c r="B424" t="s">
+      <c r="C424" t="s">
         <v>999</v>
-      </c>
-      <c r="C424" t="s">
-        <v>1000</v>
       </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A425" s="2" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B425" t="s">
         <v>1001</v>
       </c>
-      <c r="B425" t="s">
-        <v>1002</v>
-      </c>
       <c r="C425" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A426" s="2" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B426" t="s">
         <v>1003</v>
       </c>
-      <c r="B426" t="s">
+      <c r="C426" t="s">
         <v>1004</v>
-      </c>
-      <c r="C426" t="s">
-        <v>1005</v>
       </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A427" s="2" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B427" t="s">
         <v>1006</v>
       </c>
-      <c r="B427" t="s">
+      <c r="C427" t="s">
         <v>1007</v>
-      </c>
-      <c r="C427" t="s">
-        <v>1008</v>
       </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A428" s="2" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B428" t="s">
         <v>1009</v>
       </c>
-      <c r="B428" t="s">
+      <c r="C428" t="s">
         <v>1010</v>
-      </c>
-      <c r="C428" t="s">
-        <v>1011</v>
       </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A429" s="2" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B429" t="s">
         <v>1012</v>
       </c>
-      <c r="B429" t="s">
+      <c r="C429" t="s">
         <v>1013</v>
-      </c>
-      <c r="C429" t="s">
-        <v>1014</v>
       </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A430" s="2" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B430" t="s">
         <v>1015</v>
       </c>
-      <c r="B430" t="s">
+      <c r="C430" t="s">
         <v>1016</v>
-      </c>
-      <c r="C430" t="s">
-        <v>1017</v>
       </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A431" s="2" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B431" s="4" t="s">
         <v>1018</v>
       </c>
-      <c r="B431" s="4" t="s">
+      <c r="C431" t="s">
         <v>1019</v>
-      </c>
-      <c r="C431" t="s">
-        <v>1020</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A432" s="2" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B432" t="s">
         <v>1021</v>
       </c>
-      <c r="B432" t="s">
+      <c r="C432" t="s">
         <v>1022</v>
-      </c>
-      <c r="C432" t="s">
-        <v>1023</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A433" s="2" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B433" t="s">
         <v>1024</v>
       </c>
-      <c r="B433" t="s">
+      <c r="C433" t="s">
         <v>1025</v>
-      </c>
-      <c r="C433" t="s">
-        <v>1026</v>
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A434" s="2" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B434" t="s">
         <v>1027</v>
       </c>
-      <c r="B434" t="s">
+      <c r="C434" t="s">
         <v>1028</v>
-      </c>
-      <c r="C434" t="s">
-        <v>1029</v>
       </c>
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A435" s="2" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B435" t="s">
         <v>1030</v>
       </c>
-      <c r="B435" t="s">
+      <c r="C435" t="s">
         <v>1031</v>
-      </c>
-      <c r="C435" t="s">
-        <v>1032</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:C3 B1:C1 A301:C301 A300:B300 A240:C241 B239:C239 A117:C125 B15:C16 A254:C263 B253:C253 A265:C266 B264:C264 B267:C271 A303:C303 B302:C302 A309:C313 A328:C342 A314 A293:C299 A243:C252 A242 C242 A11:C12 A10 A305:C305 A304 A307:C307 A306 C306 A394:C414 A345 A5:C9 A4 A416:C435 A415:B415 A217:C230 A185:B185 A155:C184 B149:C149 A232:C238 A231 A186:C214 C152 B151:C151 C150 A17:C25 A344:C344 A343 A27:C113 A127:C148 A126:B126 A114:B114 A346:C368 A370:C391 A315:C326 A272:C291" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:C3 B1:C1 A301:C301 A300:B300 A240:C241 B239:C239 A117:C125 B15:C16 A254:C263 B253:C253 A265:C266 B264:C264 B267:C271 A303:C303 B302:C302 A309:C313 A328:C342 A314 A293:C299 A243:C252 A242 C242 A11:C12 A10 A305:C305 A304 A307:C307 A306 C306 A394:C414 A345 A5:C9 A4 A416:C416 A415:B415 A217:C230 A185:B185 A155:C184 B149:C149 A232:C238 A231 A186:C214 C152 B151:C151 C150 A17:C25 A344:C344 A343 A27:C113 A127:C148 A126:B126 A114:B114 A346:C368 A370:C391 A315:C326 A272:C291 A418:C435 A417 C417" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>